<commit_message>
switch to environment variable to check whether code runs on server or not
</commit_message>
<xml_diff>
--- a/Tests/IDA/resultIDA.xlsx
+++ b/Tests/IDA/resultIDA.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t xml:space="preserve">Model: IDA</t>
   </si>
@@ -35,7 +35,7 @@
     <t xml:space="preserve">info</t>
   </si>
   <si>
-    <t xml:space="preserve">Ka(HG) [M]</t>
+    <t xml:space="preserve">Ka(HG) [1/M]</t>
   </si>
   <si>
     <t xml:space="preserve">I(0)</t>
@@ -71,13 +71,13 @@
     <t xml:space="preserve">R2 adjusted</t>
   </si>
   <si>
-    <t xml:space="preserve">Host [M]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dye [M]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ka(HD) [1/M]</t>
+    <t xml:space="preserve">Host..M.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dye..M.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ka.HD...1.M.</t>
   </si>
   <si>
     <t xml:space="preserve">npop</t>
@@ -87,9 +87,6 @@
   </si>
   <si>
     <t xml:space="preserve">topology</t>
-  </si>
-  <si>
-    <t xml:space="preserve">error_threshold</t>
   </si>
   <si>
     <t xml:space="preserve">seed</t>
@@ -579,13 +576,13 @@
         <v>0.652593163</v>
       </c>
       <c r="C4" t="n">
-        <v>0.630967327263024</v>
+        <v>0.648529848492967</v>
       </c>
       <c r="D4" t="n">
-        <v>0.00000043425854622615</v>
+        <v>0.00000043425854624063</v>
       </c>
       <c r="E4" t="n">
-        <v>0.00000056574145377385</v>
+        <v>0.00000056574145375937</v>
       </c>
     </row>
     <row r="5">
@@ -596,13 +593,13 @@
         <v>0.625830834</v>
       </c>
       <c r="C5" t="n">
-        <v>0.605712399979771</v>
+        <v>0.622423806487813</v>
       </c>
       <c r="D5" t="n">
-        <v>0.000000466696196265237</v>
+        <v>0.000000468428447079991</v>
       </c>
       <c r="E5" t="n">
-        <v>0.000000533303803734763</v>
+        <v>0.000000531571552920009</v>
       </c>
     </row>
     <row r="6">
@@ -613,13 +610,13 @@
         <v>0.59760106</v>
       </c>
       <c r="C6" t="n">
-        <v>0.579304079224747</v>
+        <v>0.594706073172822</v>
       </c>
       <c r="D6" t="n">
-        <v>0.000000500615274992479</v>
+        <v>0.000000504707872305696</v>
       </c>
       <c r="E6" t="n">
-        <v>0.000000499384725007521</v>
+        <v>0.000000495292127694305</v>
       </c>
     </row>
     <row r="7">
@@ -630,13 +627,13 @@
         <v>0.568336413</v>
       </c>
       <c r="C7" t="n">
-        <v>0.552178020213553</v>
+        <v>0.565765582265461</v>
       </c>
       <c r="D7" t="n">
-        <v>0.000000535456223029111</v>
+        <v>0.000000542587751007786</v>
       </c>
       <c r="E7" t="n">
-        <v>0.000000464543776970889</v>
+        <v>0.000000457412248992214</v>
       </c>
     </row>
     <row r="8">
@@ -647,13 +644,13 @@
         <v>0.538605992</v>
       </c>
       <c r="C8" t="n">
-        <v>0.524865933242483</v>
+        <v>0.536147195879024</v>
       </c>
       <c r="D8" t="n">
-        <v>0.000000570536107008509</v>
+        <v>0.000000581354919376191</v>
       </c>
       <c r="E8" t="n">
-        <v>0.000000429463892991491</v>
+        <v>0.000000418645080623809</v>
       </c>
     </row>
     <row r="9">
@@ -664,13 +661,13 @@
         <v>0.509076212</v>
       </c>
       <c r="C9" t="n">
-        <v>0.497948177113512</v>
+        <v>0.506527036540974</v>
       </c>
       <c r="D9" t="n">
-        <v>0.000000605109508996804</v>
+        <v>0.000000620124408340753</v>
       </c>
       <c r="E9" t="n">
-        <v>0.000000394890491003196</v>
+        <v>0.000000379875591659247</v>
       </c>
     </row>
     <row r="10">
@@ -681,13 +678,13 @@
         <v>0.480442809</v>
       </c>
       <c r="C10" t="n">
-        <v>0.471990306536422</v>
+        <v>0.477653005296144</v>
       </c>
       <c r="D10" t="n">
-        <v>0.000000638450025565937</v>
+        <v>0.000000657917298748026</v>
       </c>
       <c r="E10" t="n">
-        <v>0.000000361549974434063</v>
+        <v>0.000000342082701251974</v>
       </c>
     </row>
     <row r="11">
@@ -698,13 +695,13 @@
         <v>0.453345361</v>
       </c>
       <c r="C11" t="n">
-        <v>0.447478161342822</v>
+        <v>0.450253924530437</v>
       </c>
       <c r="D11" t="n">
-        <v>0.000000669933639776324</v>
+        <v>0.000000693779643283786</v>
       </c>
       <c r="E11" t="n">
-        <v>0.000000330066360223677</v>
+        <v>0.000000306220356716214</v>
       </c>
     </row>
     <row r="12">
@@ -715,13 +712,13 @@
         <v>0.428286524</v>
       </c>
       <c r="C12" t="n">
-        <v>0.424768632302453</v>
+        <v>0.424936994067228</v>
       </c>
       <c r="D12" t="n">
-        <v>0.000000699101957994069</v>
+        <v>0.00000072691668501972</v>
       </c>
       <c r="E12" t="n">
-        <v>0.000000300898042005931</v>
+        <v>0.00000027308331498028</v>
       </c>
     </row>
     <row r="13">
@@ -732,13 +729,13 @@
         <v>0.40558051</v>
       </c>
       <c r="C13" t="n">
-        <v>0.404068078659885</v>
+        <v>0.402106307429678</v>
       </c>
       <c r="D13" t="n">
-        <v>0.000000725689930596082</v>
+        <v>0.000000756799510548982</v>
       </c>
       <c r="E13" t="n">
-        <v>0.000000274310069403917</v>
+        <v>0.000000243200489451018</v>
       </c>
     </row>
     <row r="14">
@@ -749,13 +746,13 @@
         <v>0.385344585</v>
       </c>
       <c r="C14" t="n">
-        <v>0.385439825846909</v>
+        <v>0.381931385321822</v>
       </c>
       <c r="D14" t="n">
-        <v>0.000000749616221842529</v>
+        <v>0.000000783206236154156</v>
       </c>
       <c r="E14" t="n">
-        <v>0.000000250383778157471</v>
+        <v>0.000000216793763845844</v>
       </c>
     </row>
     <row r="15">
@@ -766,13 +763,13 @@
         <v>0.367529159</v>
       </c>
       <c r="C15" t="n">
-        <v>0.368832416232932</v>
+        <v>0.364371701180448</v>
       </c>
       <c r="D15" t="n">
-        <v>0.000000770946924365327</v>
+        <v>0.000000806189906591935</v>
       </c>
       <c r="E15" t="n">
-        <v>0.000000229053075634673</v>
+        <v>0.000000193810093408066</v>
       </c>
     </row>
     <row r="16">
@@ -783,13 +780,13 @@
         <v>0.351968717</v>
       </c>
       <c r="C16" t="n">
-        <v>0.354116278662215</v>
+        <v>0.349237694883239</v>
       </c>
       <c r="D16" t="n">
-        <v>0.000000789848460492992</v>
+        <v>0.000000825998634945922</v>
       </c>
       <c r="E16" t="n">
-        <v>0.000000210151539507008</v>
+        <v>0.000000174001365054078</v>
       </c>
     </row>
     <row r="17">
@@ -800,13 +797,13 @@
         <v>0.338434288</v>
       </c>
       <c r="C17" t="n">
-        <v>0.341118450787961</v>
+        <v>0.336259477230041</v>
       </c>
       <c r="D17" t="n">
-        <v>0.000000806542984580295</v>
+        <v>0.000000842985676114165</v>
       </c>
       <c r="E17" t="n">
-        <v>0.000000193457015419705</v>
+        <v>0.000000157014323885836</v>
       </c>
     </row>
     <row r="18">
@@ -817,13 +814,13 @@
         <v>0.3266753</v>
       </c>
       <c r="C18" t="n">
-        <v>0.329649732510814</v>
+        <v>0.325142590763887</v>
       </c>
       <c r="D18" t="n">
-        <v>0.000000821273506893763</v>
+        <v>0.000000857536442106034</v>
       </c>
       <c r="E18" t="n">
-        <v>0.000000178726493106237</v>
+        <v>0.000000142463557893966</v>
       </c>
     </row>
     <row r="19">
@@ -834,13 +831,13 @@
         <v>0.316447156</v>
       </c>
       <c r="C19" t="n">
-        <v>0.319522969103631</v>
+        <v>0.315603831546427</v>
       </c>
       <c r="D19" t="n">
-        <v>0.000000834280410605921</v>
+        <v>0.000000870021615328647</v>
       </c>
       <c r="E19" t="n">
-        <v>0.000000165719589394079</v>
+        <v>0.000000129978384671353</v>
       </c>
     </row>
     <row r="20">
@@ -851,13 +848,13 @@
         <v>0.307526286</v>
       </c>
       <c r="C20" t="n">
-        <v>0.310563682626295</v>
+        <v>0.307389491594884</v>
       </c>
       <c r="D20" t="n">
-        <v>0.000000845787796712887</v>
+        <v>0.000000880773271269046</v>
       </c>
       <c r="E20" t="n">
-        <v>0.000000154212203287113</v>
+        <v>0.000000119226728730954</v>
       </c>
     </row>
     <row r="21">
@@ -868,13 +865,13 @@
         <v>0.299716359</v>
       </c>
       <c r="C21" t="n">
-        <v>0.302615136656782</v>
+        <v>0.300281643544003</v>
       </c>
       <c r="D21" t="n">
-        <v>0.000000855996978849383</v>
+        <v>0.000000890076652571806</v>
       </c>
       <c r="E21" t="n">
-        <v>0.000000144003021150617</v>
+        <v>0.000000109923347428194</v>
       </c>
     </row>
     <row r="22">
@@ -885,13 +882,13 @@
         <v>0.292849146</v>
       </c>
       <c r="C22" t="n">
-        <v>0.295539821073467</v>
+        <v>0.294097671648404</v>
       </c>
       <c r="D22" t="n">
-        <v>0.000000865084576221316</v>
+        <v>0.000000898170782904712</v>
       </c>
       <c r="E22" t="n">
-        <v>0.000000134915423778684</v>
+        <v>0.000000101829217095288</v>
       </c>
     </row>
     <row r="23">
@@ -902,13 +899,13 @@
         <v>0.286782597</v>
       </c>
       <c r="C23" t="n">
-        <v>0.289218878363438</v>
+        <v>0.288686655004303</v>
       </c>
       <c r="D23" t="n">
-        <v>0.000000873203250460422</v>
+        <v>0.000000905253200918617</v>
       </c>
       <c r="E23" t="n">
-        <v>0.000000126796749539578</v>
+        <v>0.0000000947467990813832</v>
       </c>
     </row>
     <row r="24">
@@ -919,13 +916,13 @@
         <v>0.281397733</v>
       </c>
       <c r="C24" t="n">
-        <v>0.283550496974634</v>
+        <v>0.283924711654066</v>
       </c>
       <c r="D24" t="n">
-        <v>0.000000880483769216856</v>
+        <v>0.000000911486054295935</v>
       </c>
       <c r="E24" t="n">
-        <v>0.000000119516230783144</v>
+        <v>0.0000000885139457040651</v>
       </c>
     </row>
     <row r="25">
@@ -936,13 +933,13 @@
         <v>0.276595271</v>
       </c>
       <c r="C25" t="n">
-        <v>0.278447901380276</v>
+        <v>0.279710377559353</v>
       </c>
       <c r="D25" t="n">
-        <v>0.000000887037587738065</v>
+        <v>0.000000917002148160025</v>
       </c>
       <c r="E25" t="n">
-        <v>0.000000112962412261935</v>
+        <v>0.0000000829978518399749</v>
       </c>
     </row>
     <row r="26">
@@ -953,13 +950,13 @@
         <v>0.272292426</v>
       </c>
       <c r="C26" t="n">
-        <v>0.273837294053258</v>
+        <v>0.275960483432322</v>
       </c>
       <c r="D26" t="n">
-        <v>0.000000892959492214925</v>
+        <v>0.000000921910341843825</v>
       </c>
       <c r="E26" t="n">
-        <v>0.000000107040507785075</v>
+        <v>0.0000000780896581561746</v>
       </c>
     </row>
     <row r="27">
@@ -970,13 +967,13 @@
         <v>0.268420086</v>
       </c>
       <c r="C27" t="n">
-        <v>0.269655930471106</v>
+        <v>0.272606669730392</v>
       </c>
       <c r="D27" t="n">
-        <v>0.000000898330072262247</v>
+        <v>0.000000926300110373503</v>
       </c>
       <c r="E27" t="n">
-        <v>0.000000101669927737753</v>
+        <v>0.0000000736998896264973</v>
       </c>
     </row>
     <row r="28">
@@ -987,13 +984,13 @@
         <v>0.264920412</v>
       </c>
       <c r="C28" t="n">
-        <v>0.26585040515474</v>
+        <v>0.269592527372223</v>
       </c>
       <c r="D28" t="n">
-        <v>0.000000903217922345626</v>
+        <v>0.000000930245286952703</v>
       </c>
       <c r="E28" t="n">
-        <v>0.000000096782077654374</v>
+        <v>0.0000000697547130472968</v>
       </c>
     </row>
     <row r="29">
@@ -1004,13 +1001,13 @@
         <v>0.261744829</v>
       </c>
       <c r="C29" t="n">
-        <v>0.262375169476971</v>
+        <v>0.26687129016102</v>
       </c>
       <c r="D29" t="n">
-        <v>0.000000907681545521194</v>
+        <v>0.000000933807083323398</v>
       </c>
       <c r="E29" t="n">
-        <v>0.0000000923184544788062</v>
+        <v>0.0000000661929166766018</v>
       </c>
     </row>
     <row r="30">
@@ -1021,13 +1018,13 @@
         <v>0.258852387</v>
       </c>
       <c r="C30" t="n">
-        <v>0.259191272567369</v>
+        <v>0.264403988435047</v>
       </c>
       <c r="D30" t="n">
-        <v>0.000000911770970628456</v>
+        <v>0.000000937036506431682</v>
       </c>
       <c r="E30" t="n">
-        <v>0.0000000882290293715444</v>
+        <v>0.0000000629634935683178</v>
       </c>
     </row>
     <row r="31">
@@ -1038,13 +1035,13 @@
         <v>0.256208419</v>
       </c>
       <c r="C31" t="n">
-        <v>0.256265303329095</v>
+        <v>0.262157977234234</v>
       </c>
       <c r="D31" t="n">
-        <v>0.000000915529111173141</v>
+        <v>0.000000939976284893723</v>
       </c>
       <c r="E31" t="n">
-        <v>0.0000000844708888268592</v>
+        <v>0.0000000600237151062767</v>
       </c>
     </row>
     <row r="32">
@@ -1055,13 +1052,13 @@
         <v>0.253783444</v>
       </c>
       <c r="C32" t="n">
-        <v>0.25356850712089</v>
+        <v>0.260105763679687</v>
       </c>
       <c r="D32" t="n">
-        <v>0.000000918992899868604</v>
+        <v>0.000000942662403825356</v>
       </c>
       <c r="E32" t="n">
-        <v>0.0000000810071001313955</v>
+        <v>0.0000000573375961746439</v>
       </c>
     </row>
     <row r="33">
@@ -1072,13 +1069,13 @@
         <v>0.251552283</v>
       </c>
       <c r="C33" t="n">
-        <v>0.251076050762459</v>
+        <v>0.258224071347308</v>
       </c>
       <c r="D33" t="n">
-        <v>0.000000922194232669356</v>
+        <v>0.000000945125329472794</v>
       </c>
       <c r="E33" t="n">
-        <v>0.0000000778057673306437</v>
+        <v>0.0000000548746705272058</v>
       </c>
     </row>
     <row r="34">
@@ -1089,13 +1086,13 @@
         <v>0.249493336</v>
       </c>
       <c r="C34" t="n">
-        <v>0.248766411759554</v>
+        <v>0.256493091619655</v>
       </c>
       <c r="D34" t="n">
-        <v>0.000000925160753255719</v>
+        <v>0.000000947390989109638</v>
       </c>
       <c r="E34" t="n">
-        <v>0.0000000748392467442812</v>
+        <v>0.0000000526090108903618</v>
       </c>
     </row>
     <row r="35">
@@ -1106,13 +1103,13 @@
         <v>0.24758799</v>
       </c>
       <c r="C35" t="n">
-        <v>0.246620870685677</v>
+        <v>0.254895882425806</v>
       </c>
       <c r="D35" t="n">
-        <v>0.000000927916505023218</v>
+        <v>0.000000949481558019424</v>
       </c>
       <c r="E35" t="n">
-        <v>0.0000000720834949767818</v>
+        <v>0.0000000505184419805758</v>
       </c>
     </row>
     <row r="36">
@@ -1123,13 +1120,13 @@
         <v>0.245820143</v>
       </c>
       <c r="C36" t="n">
-        <v>0.244623088810315</v>
+        <v>0.253417883292073</v>
       </c>
       <c r="D36" t="n">
-        <v>0.000000930482473580586</v>
+        <v>0.000000951416094240209</v>
       </c>
       <c r="E36" t="n">
-        <v>0.0000000695175264194141</v>
+        <v>0.0000000485839057597909</v>
       </c>
     </row>
     <row r="37">
@@ -1140,13 +1137,13 @@
         <v>0.244175803</v>
       </c>
       <c r="C37" t="n">
-        <v>0.242758755999274</v>
+        <v>0.25204652240452</v>
       </c>
       <c r="D37" t="n">
-        <v>0.000000932877038989651</v>
+        <v>0.00000095321105287597</v>
       </c>
       <c r="E37" t="n">
-        <v>0.0000000671229610103484</v>
+        <v>0.0000000467889471240304</v>
       </c>
     </row>
     <row r="38">
@@ -1157,13 +1154,13 @@
         <v>0.242642769</v>
       </c>
       <c r="C38" t="n">
-        <v>0.241015296497869</v>
+        <v>0.250770896703734</v>
       </c>
       <c r="D38" t="n">
-        <v>0.000000935116353659996</v>
+        <v>0.000000954880704816902</v>
       </c>
       <c r="E38" t="n">
-        <v>0.0000000648836463400038</v>
+        <v>0.0000000451192951830974</v>
       </c>
     </row>
     <row r="39">
@@ -1174,13 +1171,13 @@
         <v>0.241210354</v>
       </c>
       <c r="C39" t="n">
-        <v>0.239381622411708</v>
+        <v>0.249581510174421</v>
       </c>
       <c r="D39" t="n">
-        <v>0.000000937214658980399</v>
+        <v>0.000000956437479289199</v>
       </c>
       <c r="E39" t="n">
-        <v>0.0000000627853410196008</v>
+        <v>0.000000043562520710801</v>
       </c>
     </row>
     <row r="40">
@@ -1191,13 +1188,13 @@
         <v>0.23986917</v>
       </c>
       <c r="C40" t="n">
-        <v>0.237847926541777</v>
+        <v>0.248470058705374</v>
       </c>
       <c r="D40" t="n">
-        <v>0.00000093918455140326</v>
+        <v>0.00000095789224544937</v>
       </c>
       <c r="E40" t="n">
-        <v>0.0000000608154485967399</v>
+        <v>0.0000000421077545506306</v>
       </c>
     </row>
     <row r="41">
@@ -1208,13 +1205,13 @@
         <v>0.238610935</v>
       </c>
       <c r="C41" t="n">
-        <v>0.236405507750851</v>
+        <v>0.247429252385031</v>
       </c>
       <c r="D41" t="n">
-        <v>0.000000941037206745527</v>
+        <v>0.000000959254544979573</v>
       </c>
       <c r="E41" t="n">
-        <v>0.0000000589627932544731</v>
+        <v>0.0000000407454550204266</v>
       </c>
     </row>
     <row r="42">
@@ -1225,13 +1222,13 @@
         <v>0.237428323</v>
       </c>
       <c r="C42" t="n">
-        <v>0.235046623283152</v>
+        <v>0.246452668028221</v>
       </c>
       <c r="D42" t="n">
-        <v>0.000000942782569870607</v>
+        <v>0.000000960532785113672</v>
       </c>
       <c r="E42" t="n">
-        <v>0.0000000572174301293925</v>
+        <v>0.0000000394672148863274</v>
       </c>
     </row>
     <row r="43">
@@ -1242,13 +1239,13 @@
         <v>0.236314829</v>
       </c>
       <c r="C43" t="n">
-        <v>0.233764363474007</v>
+        <v>0.245534626229506</v>
       </c>
       <c r="D43" t="n">
-        <v>0.000000944429515612391</v>
+        <v>0.000000961734399560715</v>
       </c>
       <c r="E43" t="n">
-        <v>0.0000000555704843876085</v>
+        <v>0.000000038265600439285</v>
       </c>
     </row>
     <row r="44">
@@ -1259,13 +1256,13 @@
         <v>0.235264662</v>
       </c>
       <c r="C44" t="n">
-        <v>0.232552545111203</v>
+        <v>0.244670088406896</v>
       </c>
       <c r="D44" t="n">
-        <v>0.000000945985985742862</v>
+        <v>0.00000096286598326324</v>
       </c>
       <c r="E44" t="n">
-        <v>0.0000000540140142571387</v>
+        <v>0.0000000371340167367604</v>
       </c>
     </row>
     <row r="45">
@@ -1276,13 +1273,13 @@
         <v>0.23427265</v>
       </c>
       <c r="C45" t="n">
-        <v>0.23140562037983</v>
+        <v>0.243854570213064</v>
       </c>
       <c r="D45" t="n">
-        <v>0.00000094745910592413</v>
+        <v>0.000000963933405732354</v>
       </c>
       <c r="E45" t="n">
-        <v>0.0000000525408940758694</v>
+        <v>0.0000000360665942676465</v>
       </c>
     </row>
     <row r="46">
@@ -1293,13 +1290,13 @@
         <v>0.23333416</v>
       </c>
       <c r="C46" t="n">
-        <v>0.230318598866684</v>
+        <v>0.243084068407775</v>
       </c>
       <c r="D46" t="n">
-        <v>0.000000948855285886676</v>
+        <v>0.000000964941906763574</v>
       </c>
       <c r="E46" t="n">
-        <v>0.0000000511447141133245</v>
+        <v>0.0000000350580932364263</v>
       </c>
     </row>
     <row r="47">
@@ -1310,13 +1307,13 @@
         <v>0.232445033</v>
       </c>
       <c r="C47" t="n">
-        <v>0.22928698054278</v>
+        <v>0.24235499884977</v>
       </c>
       <c r="D47" t="n">
-        <v>0.000000950180305507179</v>
+        <v>0.000000965896177598544</v>
       </c>
       <c r="E47" t="n">
-        <v>0.0000000498196944928212</v>
+        <v>0.0000000341038224014562</v>
       </c>
     </row>
     <row r="48">
@@ -1327,13 +1324,13 @@
         <v>0.231601522</v>
       </c>
       <c r="C48" t="n">
-        <v>0.228306698002824</v>
+        <v>0.241664143712879</v>
       </c>
       <c r="D48" t="n">
-        <v>0.000000951439388996665</v>
+        <v>0.000000966800430013264</v>
       </c>
       <c r="E48" t="n">
-        <v>0.0000000485606110033347</v>
+        <v>0.0000000331995699867362</v>
       </c>
     </row>
     <row r="49">
@@ -1344,13 +1341,13 @@
         <v>0.230800248</v>
       </c>
       <c r="C49" t="n">
-        <v>0.227374066534354</v>
+        <v>0.241008606385855</v>
       </c>
       <c r="D49" t="n">
-        <v>0.000000952637269032128</v>
+        <v>0.000000967658455349179</v>
       </c>
       <c r="E49" t="n">
-        <v>0.0000000473627309678719</v>
+        <v>0.0000000323415446508204</v>
       </c>
     </row>
     <row r="50">
@@ -1361,13 +1358,13 @@
         <v>0.230038151</v>
       </c>
       <c r="C50" t="n">
-        <v>0.226485740829573</v>
+        <v>0.240385772798418</v>
       </c>
       <c r="D50" t="n">
-        <v>0.000000953778242356233</v>
+        <v>0.000000968473675133087</v>
       </c>
       <c r="E50" t="n">
-        <v>0.0000000462217576437673</v>
+        <v>0.000000031526324866913</v>
       </c>
     </row>
     <row r="51">
@@ -1378,13 +1375,13 @@
         <v>0.229312458</v>
       </c>
       <c r="C51" t="n">
-        <v>0.22563867734979</v>
+        <v>0.239793278142695</v>
       </c>
       <c r="D51" t="n">
-        <v>0.000000954866218116762</v>
+        <v>0.000000969249184635061</v>
       </c>
       <c r="E51" t="n">
-        <v>0.0000000451337818832377</v>
+        <v>0.0000000307508153649391</v>
       </c>
     </row>
     <row r="52">
@@ -1395,13 +1392,13 @@
         <v>0.228620648</v>
       </c>
       <c r="C52" t="n">
-        <v>0.224830101514185</v>
+        <v>0.239228978141636</v>
       </c>
       <c r="D52" t="n">
-        <v>0.000000955904760009647</v>
+        <v>0.000000969987790474891</v>
       </c>
       <c r="E52" t="n">
-        <v>0.000000044095239990353</v>
+        <v>0.0000000300122095251094</v>
       </c>
     </row>
     <row r="53">
@@ -1412,13 +1409,13 @@
         <v>0.227960426</v>
       </c>
       <c r="C53" t="n">
-        <v>0.224057479017966</v>
+        <v>0.238690924163362</v>
       </c>
       <c r="D53" t="n">
-        <v>0.000000956897123118184</v>
+        <v>0.000000970692043194632</v>
       </c>
       <c r="E53" t="n">
-        <v>0.0000000431028768818161</v>
+        <v>0.0000000293079568053678</v>
       </c>
     </row>
     <row r="54">
@@ -1429,13 +1426,13 @@
         <v>0.227329698</v>
       </c>
       <c r="C54" t="n">
-        <v>0.223318490695077</v>
+        <v>0.238177341599896</v>
       </c>
       <c r="D54" t="n">
-        <v>0.000000957846286199589</v>
+        <v>0.000000971364265558444</v>
       </c>
       <c r="E54" t="n">
-        <v>0.0000000421537138004109</v>
+        <v>0.0000000286357344415556</v>
       </c>
     </row>
     <row r="59">
@@ -1460,16 +1457,16 @@
         <v>11</v>
       </c>
       <c r="B60" t="n">
-        <v>15848500.8011864</v>
+        <v>24229546.9940493</v>
       </c>
       <c r="C60" t="n">
         <v>0.000000000000001</v>
       </c>
       <c r="D60" t="n">
-        <v>969067.281910087</v>
+        <v>980306.399515205</v>
       </c>
       <c r="E60" t="n">
-        <v>190498.94379616</v>
+        <v>216299.441230966</v>
       </c>
     </row>
     <row r="61">
@@ -1525,19 +1522,19 @@
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>0.0000419371374905922</v>
+        <v>0.0000431811411794888</v>
       </c>
       <c r="B68" t="n">
-        <v>0.00647588893439288</v>
+        <v>0.00657123589437245</v>
       </c>
       <c r="C68" t="n">
-        <v>0.00406907024414551</v>
+        <v>0.00568664148842454</v>
       </c>
       <c r="D68" t="n">
-        <v>0.998874948560538</v>
+        <v>0.999271523493237</v>
       </c>
       <c r="E68" t="n">
-        <v>0.99885198832708</v>
+        <v>0.999256656625752</v>
       </c>
     </row>
     <row r="88">
@@ -1562,9 +1559,6 @@
       <c r="G88" t="s">
         <v>25</v>
       </c>
-      <c r="H88" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
@@ -1580,109 +1574,106 @@
         <v>40</v>
       </c>
       <c r="E89" t="n">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="F89" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G89" t="n">
-        <v>0.00001</v>
-      </c>
-      <c r="H89" t="n">
         <v>1234</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s">
+        <v>27</v>
+      </c>
+      <c r="B93" t="s">
         <v>28</v>
       </c>
-      <c r="B93" t="s">
+      <c r="C93" t="s">
         <v>29</v>
       </c>
-      <c r="C93" t="s">
+      <c r="D93" t="s">
         <v>30</v>
       </c>
-      <c r="D93" t="s">
+      <c r="E93" t="s">
         <v>31</v>
       </c>
-      <c r="E93" t="s">
+      <c r="F93" t="s">
         <v>32</v>
       </c>
-      <c r="F93" t="s">
+      <c r="G93" t="s">
         <v>33</v>
       </c>
-      <c r="G93" t="s">
+      <c r="H93" t="s">
         <v>34</v>
       </c>
-      <c r="H93" t="s">
+      <c r="I93" t="s">
         <v>35</v>
       </c>
-      <c r="I93" t="s">
+      <c r="J93" t="s">
         <v>36</v>
       </c>
-      <c r="J93" t="s">
+      <c r="K93" t="s">
         <v>37</v>
       </c>
-      <c r="K93" t="s">
+      <c r="L93" t="s">
         <v>38</v>
       </c>
-      <c r="L93" t="s">
+      <c r="M93" t="s">
         <v>39</v>
       </c>
-      <c r="M93" t="s">
+      <c r="N93" t="s">
         <v>40</v>
-      </c>
-      <c r="N93" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s">
+        <v>41</v>
+      </c>
+      <c r="B94" t="s">
         <v>42</v>
       </c>
-      <c r="B94" t="s">
+      <c r="C94" t="s">
         <v>43</v>
       </c>
-      <c r="C94" t="s">
+      <c r="D94" t="s">
         <v>44</v>
       </c>
-      <c r="D94" t="s">
+      <c r="E94" t="s">
         <v>45</v>
       </c>
-      <c r="E94" t="s">
+      <c r="F94" t="s">
         <v>46</v>
       </c>
-      <c r="F94" t="s">
+      <c r="G94" t="s">
         <v>47</v>
       </c>
-      <c r="G94" t="s">
+      <c r="H94" t="s">
         <v>48</v>
       </c>
-      <c r="H94" t="s">
+      <c r="I94" t="s">
         <v>49</v>
       </c>
-      <c r="I94" t="s">
+      <c r="J94" t="s">
         <v>50</v>
       </c>
-      <c r="J94" t="s">
+      <c r="K94" t="s">
         <v>51</v>
       </c>
-      <c r="K94" t="s">
+      <c r="L94" t="s">
         <v>52</v>
       </c>
-      <c r="L94" t="s">
+      <c r="M94" t="s">
         <v>53</v>
       </c>
-      <c r="M94" t="s">
+      <c r="N94" t="s">
         <v>54</v>
-      </c>
-      <c r="N94" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added a new UI test for IDA
</commit_message>
<xml_diff>
--- a/Tests/IDA/resultIDA.xlsx
+++ b/Tests/IDA/resultIDA.xlsx
@@ -576,13 +576,13 @@
         <v>0.652593163</v>
       </c>
       <c r="C4" t="n">
-        <v>0.648529848492967</v>
+        <v>0.647493714776973</v>
       </c>
       <c r="D4" t="n">
-        <v>0.00000043425854624063</v>
+        <v>0.000000434258546210193</v>
       </c>
       <c r="E4" t="n">
-        <v>0.00000056574145375937</v>
+        <v>0.000000565741453789807</v>
       </c>
     </row>
     <row r="5">
@@ -593,13 +593,13 @@
         <v>0.625830834</v>
       </c>
       <c r="C5" t="n">
-        <v>0.622423806487813</v>
+        <v>0.621839150372756</v>
       </c>
       <c r="D5" t="n">
-        <v>0.000000468428447079991</v>
+        <v>0.000000464836856958639</v>
       </c>
       <c r="E5" t="n">
-        <v>0.000000531571552920009</v>
+        <v>0.000000535163143041362</v>
       </c>
     </row>
     <row r="6">
@@ -610,13 +610,13 @@
         <v>0.59760106</v>
       </c>
       <c r="C6" t="n">
-        <v>0.594706073172822</v>
+        <v>0.595399314904643</v>
       </c>
       <c r="D6" t="n">
-        <v>0.000000504707872305696</v>
+        <v>0.000000496351151738434</v>
       </c>
       <c r="E6" t="n">
-        <v>0.000000495292127694305</v>
+        <v>0.000000503648848261566</v>
       </c>
     </row>
     <row r="7">
@@ -627,13 +627,13 @@
         <v>0.568336413</v>
       </c>
       <c r="C7" t="n">
-        <v>0.565765582265461</v>
+        <v>0.56862717406658</v>
       </c>
       <c r="D7" t="n">
-        <v>0.000000542587751007786</v>
+        <v>0.000000528261529519507</v>
       </c>
       <c r="E7" t="n">
-        <v>0.000000457412248992214</v>
+        <v>0.000000471738470480493</v>
       </c>
     </row>
     <row r="8">
@@ -644,13 +644,13 @@
         <v>0.538605992</v>
       </c>
       <c r="C8" t="n">
-        <v>0.536147195879024</v>
+        <v>0.542017511793281</v>
       </c>
       <c r="D8" t="n">
-        <v>0.000000581354919376191</v>
+        <v>0.000000559978245074825</v>
       </c>
       <c r="E8" t="n">
-        <v>0.000000418645080623809</v>
+        <v>0.000000440021754925175</v>
       </c>
     </row>
     <row r="9">
@@ -661,13 +661,13 @@
         <v>0.509076212</v>
       </c>
       <c r="C9" t="n">
-        <v>0.506527036540974</v>
+        <v>0.51605709427587</v>
       </c>
       <c r="D9" t="n">
-        <v>0.000000620124408340753</v>
+        <v>0.000000590921109724527</v>
       </c>
       <c r="E9" t="n">
-        <v>0.000000379875591659247</v>
+        <v>0.000000409078890275473</v>
       </c>
     </row>
     <row r="10">
@@ -678,13 +678,13 @@
         <v>0.480442809</v>
       </c>
       <c r="C10" t="n">
-        <v>0.477653005296144</v>
+        <v>0.491175476371241</v>
       </c>
       <c r="D10" t="n">
-        <v>0.000000657917298748026</v>
+        <v>0.000000620578126395088</v>
       </c>
       <c r="E10" t="n">
-        <v>0.000000342082701251974</v>
+        <v>0.000000379421873604912</v>
       </c>
     </row>
     <row r="11">
@@ -695,13 +695,13 @@
         <v>0.453345361</v>
       </c>
       <c r="C11" t="n">
-        <v>0.450253924530437</v>
+        <v>0.467707953921521</v>
       </c>
       <c r="D11" t="n">
-        <v>0.000000693779643283786</v>
+        <v>0.000000648549647667369</v>
       </c>
       <c r="E11" t="n">
-        <v>0.000000306220356716214</v>
+        <v>0.000000351450352332631</v>
       </c>
     </row>
     <row r="12">
@@ -712,13 +712,13 @@
         <v>0.428286524</v>
       </c>
       <c r="C12" t="n">
-        <v>0.424936994067228</v>
+        <v>0.445877659860333</v>
       </c>
       <c r="D12" t="n">
-        <v>0.00000072691668501972</v>
+        <v>0.00000067456971587103</v>
       </c>
       <c r="E12" t="n">
-        <v>0.00000027308331498028</v>
+        <v>0.00000032543028412897</v>
       </c>
     </row>
     <row r="13">
@@ -729,13 +729,13 @@
         <v>0.40558051</v>
       </c>
       <c r="C13" t="n">
-        <v>0.402106307429678</v>
+        <v>0.425797141956223</v>
       </c>
       <c r="D13" t="n">
-        <v>0.000000756799510548982</v>
+        <v>0.000000698504182533059</v>
       </c>
       <c r="E13" t="n">
-        <v>0.000000243200489451018</v>
+        <v>0.000000301495817466941</v>
       </c>
     </row>
     <row r="14">
@@ -746,13 +746,13 @@
         <v>0.385344585</v>
       </c>
       <c r="C14" t="n">
-        <v>0.381931385321822</v>
+        <v>0.407484352082496</v>
       </c>
       <c r="D14" t="n">
-        <v>0.000000783206236154156</v>
+        <v>0.000000720331650371015</v>
       </c>
       <c r="E14" t="n">
-        <v>0.000000216793763845844</v>
+        <v>0.000000279668349628985</v>
       </c>
     </row>
     <row r="15">
@@ -763,13 +763,13 @@
         <v>0.367529159</v>
       </c>
       <c r="C15" t="n">
-        <v>0.364371701180448</v>
+        <v>0.390885811325673</v>
       </c>
       <c r="D15" t="n">
-        <v>0.000000806189906591935</v>
+        <v>0.000000740115862226487</v>
       </c>
       <c r="E15" t="n">
-        <v>0.000000193810093408066</v>
+        <v>0.000000259884137773513</v>
       </c>
     </row>
     <row r="16">
@@ -780,13 +780,13 @@
         <v>0.351968717</v>
       </c>
       <c r="C16" t="n">
-        <v>0.349237694883239</v>
+        <v>0.375900564325419</v>
       </c>
       <c r="D16" t="n">
-        <v>0.000000825998634945922</v>
+        <v>0.00000075797714929401</v>
       </c>
       <c r="E16" t="n">
-        <v>0.000000174001365054078</v>
+        <v>0.00000024202285070599</v>
       </c>
     </row>
     <row r="17">
@@ -797,13 +797,13 @@
         <v>0.338434288</v>
       </c>
       <c r="C17" t="n">
-        <v>0.336259477230041</v>
+        <v>0.362400882534459</v>
       </c>
       <c r="D17" t="n">
-        <v>0.000000842985676114165</v>
+        <v>0.000000774067754392775</v>
       </c>
       <c r="E17" t="n">
-        <v>0.000000157014323885836</v>
+        <v>0.000000225932245607225</v>
       </c>
     </row>
     <row r="18">
@@ -814,13 +814,13 @@
         <v>0.3266753</v>
       </c>
       <c r="C18" t="n">
-        <v>0.325142590763887</v>
+        <v>0.350248050006679</v>
       </c>
       <c r="D18" t="n">
-        <v>0.000000857536442106034</v>
+        <v>0.000000788553016494796</v>
       </c>
       <c r="E18" t="n">
-        <v>0.000000142463557893966</v>
+        <v>0.000000211446983505204</v>
       </c>
     </row>
     <row r="19">
@@ -831,13 +831,13 @@
         <v>0.316447156</v>
       </c>
       <c r="C19" t="n">
-        <v>0.315603831546427</v>
+        <v>0.33930321517537</v>
       </c>
       <c r="D19" t="n">
-        <v>0.000000870021615328647</v>
+        <v>0.000000801598436221633</v>
       </c>
       <c r="E19" t="n">
-        <v>0.000000129978384671353</v>
+        <v>0.000000198401563778367</v>
       </c>
     </row>
     <row r="20">
@@ -848,13 +848,13 @@
         <v>0.307526286</v>
       </c>
       <c r="C20" t="n">
-        <v>0.307389491594884</v>
+        <v>0.329434124050825</v>
       </c>
       <c r="D20" t="n">
-        <v>0.000000880773271269046</v>
+        <v>0.000000813361650379402</v>
       </c>
       <c r="E20" t="n">
-        <v>0.000000119226728730954</v>
+        <v>0.000000186638349620598</v>
       </c>
     </row>
     <row r="21">
@@ -865,13 +865,13 @@
         <v>0.299716359</v>
       </c>
       <c r="C21" t="n">
-        <v>0.300281643544003</v>
+        <v>0.320518789466025</v>
       </c>
       <c r="D21" t="n">
-        <v>0.000000890076652571806</v>
+        <v>0.000000823988058493958</v>
       </c>
       <c r="E21" t="n">
-        <v>0.000000109923347428194</v>
+        <v>0.000000176011941506042</v>
       </c>
     </row>
     <row r="22">
@@ -882,13 +882,13 @@
         <v>0.292849146</v>
       </c>
       <c r="C22" t="n">
-        <v>0.294097671648404</v>
+        <v>0.312447069022085</v>
       </c>
       <c r="D22" t="n">
-        <v>0.000000898170782904712</v>
+        <v>0.000000833608942018638</v>
       </c>
       <c r="E22" t="n">
-        <v>0.000000101829217095288</v>
+        <v>0.000000166391057981362</v>
       </c>
     </row>
     <row r="23">
@@ -899,13 +899,13 @@
         <v>0.286782597</v>
       </c>
       <c r="C23" t="n">
-        <v>0.288686655004303</v>
+        <v>0.305120919942014</v>
       </c>
       <c r="D23" t="n">
-        <v>0.000000905253200918617</v>
+        <v>0.000000842341160567748</v>
       </c>
       <c r="E23" t="n">
-        <v>0.0000000947467990813832</v>
+        <v>0.000000157658839432251</v>
       </c>
     </row>
     <row r="24">
@@ -916,13 +916,13 @@
         <v>0.281397733</v>
       </c>
       <c r="C24" t="n">
-        <v>0.283924711654066</v>
+        <v>0.298453882563584</v>
       </c>
       <c r="D24" t="n">
-        <v>0.000000911486054295935</v>
+        <v>0.000000850287767554208</v>
       </c>
       <c r="E24" t="n">
-        <v>0.0000000885139457040651</v>
+        <v>0.000000149712232445792</v>
       </c>
     </row>
     <row r="25">
@@ -933,13 +933,13 @@
         <v>0.276595271</v>
       </c>
       <c r="C25" t="n">
-        <v>0.279710377559353</v>
+        <v>0.292370162441184</v>
       </c>
       <c r="D25" t="n">
-        <v>0.000000917002148160025</v>
+        <v>0.000000857539104255085</v>
       </c>
       <c r="E25" t="n">
-        <v>0.0000000829978518399749</v>
+        <v>0.000000142460895744915</v>
       </c>
     </row>
     <row r="26">
@@ -950,13 +950,13 @@
         <v>0.272292426</v>
       </c>
       <c r="C26" t="n">
-        <v>0.275960483432322</v>
+        <v>0.286803545256288</v>
       </c>
       <c r="D26" t="n">
-        <v>0.000000921910341843825</v>
+        <v>0.000000864174093156687</v>
       </c>
       <c r="E26" t="n">
-        <v>0.0000000780896581561746</v>
+        <v>0.000000135825906843313</v>
       </c>
     </row>
     <row r="27">
@@ -967,13 +967,13 @@
         <v>0.268420086</v>
       </c>
       <c r="C27" t="n">
-        <v>0.272606669730392</v>
+        <v>0.281696284486831</v>
       </c>
       <c r="D27" t="n">
-        <v>0.000000926300110373503</v>
+        <v>0.000000870261563768977</v>
       </c>
       <c r="E27" t="n">
-        <v>0.0000000736998896264973</v>
+        <v>0.000000129738436231023</v>
       </c>
     </row>
     <row r="28">
@@ -984,13 +984,13 @@
         <v>0.264920412</v>
       </c>
       <c r="C28" t="n">
-        <v>0.269592527372223</v>
+        <v>0.276998039730197</v>
       </c>
       <c r="D28" t="n">
-        <v>0.000000930245286952703</v>
+        <v>0.000000875861518064712</v>
       </c>
       <c r="E28" t="n">
-        <v>0.0000000697547130472968</v>
+        <v>0.000000124138481935288</v>
       </c>
     </row>
     <row r="29">
@@ -1001,13 +1001,13 @@
         <v>0.261744829</v>
       </c>
       <c r="C29" t="n">
-        <v>0.26687129016102</v>
+        <v>0.272664904464324</v>
       </c>
       <c r="D29" t="n">
-        <v>0.000000933807083323398</v>
+        <v>0.000000881026289315054</v>
       </c>
       <c r="E29" t="n">
-        <v>0.0000000661929166766018</v>
+        <v>0.000000118973710684946</v>
       </c>
     </row>
     <row r="30">
@@ -1018,13 +1018,13 @@
         <v>0.258852387</v>
       </c>
       <c r="C30" t="n">
-        <v>0.264403988435047</v>
+        <v>0.268658538404631</v>
       </c>
       <c r="D30" t="n">
-        <v>0.000000937036506431682</v>
+        <v>0.000000885801576254837</v>
       </c>
       <c r="E30" t="n">
-        <v>0.0000000629634935683178</v>
+        <v>0.000000114198423745163</v>
       </c>
     </row>
     <row r="31">
@@ -1035,13 +1035,13 @@
         <v>0.256208419</v>
       </c>
       <c r="C31" t="n">
-        <v>0.262157977234234</v>
+        <v>0.264945406025589</v>
       </c>
       <c r="D31" t="n">
-        <v>0.000000939976284893723</v>
+        <v>0.000000890227350707582</v>
       </c>
       <c r="E31" t="n">
-        <v>0.0000000600237151062767</v>
+        <v>0.000000109772649292419</v>
       </c>
     </row>
     <row r="32">
@@ -1052,13 +1052,13 @@
         <v>0.253783444</v>
       </c>
       <c r="C32" t="n">
-        <v>0.260105763679687</v>
+        <v>0.261496115522168</v>
       </c>
       <c r="D32" t="n">
-        <v>0.000000942662403825356</v>
+        <v>0.000000894338645493703</v>
       </c>
       <c r="E32" t="n">
-        <v>0.0000000573375961746439</v>
+        <v>0.000000105661354506296</v>
       </c>
     </row>
     <row r="33">
@@ -1069,13 +1069,13 @@
         <v>0.251552283</v>
       </c>
       <c r="C33" t="n">
-        <v>0.258224071347308</v>
+        <v>0.258284849017599</v>
       </c>
       <c r="D33" t="n">
-        <v>0.000000945125329472794</v>
+        <v>0.000000898166233580003</v>
       </c>
       <c r="E33" t="n">
-        <v>0.0000000548746705272058</v>
+        <v>0.000000101833766419997</v>
       </c>
     </row>
     <row r="34">
@@ -1086,13 +1086,13 @@
         <v>0.249493336</v>
       </c>
       <c r="C34" t="n">
-        <v>0.256493091619655</v>
+        <v>0.255288873597191</v>
       </c>
       <c r="D34" t="n">
-        <v>0.000000947390989109638</v>
+        <v>0.000000901737210890569</v>
       </c>
       <c r="E34" t="n">
-        <v>0.0000000526090108903618</v>
+        <v>0.0000000982627891094308</v>
       </c>
     </row>
     <row r="35">
@@ -1103,13 +1103,13 @@
         <v>0.24758799</v>
       </c>
       <c r="C35" t="n">
-        <v>0.254895882425806</v>
+        <v>0.252488122774952</v>
       </c>
       <c r="D35" t="n">
-        <v>0.000000949481558019424</v>
+        <v>0.000000905075495167083</v>
       </c>
       <c r="E35" t="n">
-        <v>0.0000000505184419805758</v>
+        <v>0.0000000949245048329171</v>
       </c>
     </row>
     <row r="36">
@@ -1120,13 +1120,13 @@
         <v>0.245820143</v>
       </c>
       <c r="C36" t="n">
-        <v>0.253417883292073</v>
+        <v>0.24986483867775</v>
       </c>
       <c r="D36" t="n">
-        <v>0.000000951416094240209</v>
+        <v>0.00000090820225245837</v>
       </c>
       <c r="E36" t="n">
-        <v>0.0000000485839057597909</v>
+        <v>0.0000000917977475416296</v>
       </c>
     </row>
     <row r="37">
@@ -1137,13 +1137,13 @@
         <v>0.244175803</v>
       </c>
       <c r="C37" t="n">
-        <v>0.25204652240452</v>
+        <v>0.247403266202889</v>
       </c>
       <c r="D37" t="n">
-        <v>0.00000095321105287597</v>
+        <v>0.000000911136261661573</v>
       </c>
       <c r="E37" t="n">
-        <v>0.0000000467889471240304</v>
+        <v>0.0000000888637383384268</v>
       </c>
     </row>
     <row r="38">
@@ -1154,13 +1154,13 @@
         <v>0.242642769</v>
       </c>
       <c r="C38" t="n">
-        <v>0.250770896703734</v>
+        <v>0.245089391463965</v>
       </c>
       <c r="D38" t="n">
-        <v>0.000000954880704816902</v>
+        <v>0.000000913894226275003</v>
       </c>
       <c r="E38" t="n">
-        <v>0.0000000451192951830974</v>
+        <v>0.0000000861057737249968</v>
       </c>
     </row>
     <row r="39">
@@ -1171,13 +1171,13 @@
         <v>0.241210354</v>
       </c>
       <c r="C39" t="n">
-        <v>0.249581510174421</v>
+        <v>0.24291071787482</v>
       </c>
       <c r="D39" t="n">
-        <v>0.000000956437479289199</v>
+        <v>0.000000916491041289229</v>
       </c>
       <c r="E39" t="n">
-        <v>0.000000043562520710801</v>
+        <v>0.0000000835089587107709</v>
       </c>
     </row>
     <row r="40">
@@ -1188,13 +1188,13 @@
         <v>0.23986917</v>
       </c>
       <c r="C40" t="n">
-        <v>0.248470058705374</v>
+        <v>0.240856074176031</v>
       </c>
       <c r="D40" t="n">
-        <v>0.00000095789224544937</v>
+        <v>0.000000918940022005058</v>
       </c>
       <c r="E40" t="n">
-        <v>0.0000000421077545506306</v>
+        <v>0.0000000810599779949423</v>
       </c>
     </row>
     <row r="41">
@@ -1205,13 +1205,13 @@
         <v>0.238610935</v>
       </c>
       <c r="C41" t="n">
-        <v>0.247429252385031</v>
+        <v>0.238915449559289</v>
       </c>
       <c r="D41" t="n">
-        <v>0.000000959254544979573</v>
+        <v>0.000000921253100552868</v>
       </c>
       <c r="E41" t="n">
-        <v>0.0000000407454550204266</v>
+        <v>0.0000000787468994471322</v>
       </c>
     </row>
     <row r="42">
@@ -1222,13 +1222,13 @@
         <v>0.237428323</v>
       </c>
       <c r="C42" t="n">
-        <v>0.246452668028221</v>
+        <v>0.237079851787031</v>
       </c>
       <c r="D42" t="n">
-        <v>0.000000960532785113672</v>
+        <v>0.000000923440995003341</v>
       </c>
       <c r="E42" t="n">
-        <v>0.0000000394672148863274</v>
+        <v>0.0000000765590049966593</v>
       </c>
     </row>
     <row r="43">
@@ -1239,13 +1239,13 @@
         <v>0.236314829</v>
       </c>
       <c r="C43" t="n">
-        <v>0.245534626229506</v>
+        <v>0.235341184842434</v>
       </c>
       <c r="D43" t="n">
-        <v>0.000000961734399560715</v>
+        <v>0.000000925513355199454</v>
       </c>
       <c r="E43" t="n">
-        <v>0.000000038265600439285</v>
+        <v>0.0000000744866448005456</v>
       </c>
     </row>
     <row r="44">
@@ -1256,13 +1256,13 @@
         <v>0.235264662</v>
       </c>
       <c r="C44" t="n">
-        <v>0.244670088406896</v>
+        <v>0.233692143187805</v>
       </c>
       <c r="D44" t="n">
-        <v>0.00000096286598326324</v>
+        <v>0.000000927478888792536</v>
       </c>
       <c r="E44" t="n">
-        <v>0.0000000371340167367604</v>
+        <v>0.0000000725211112074643</v>
       </c>
     </row>
     <row r="45">
@@ -1273,13 +1273,13 @@
         <v>0.23427265</v>
       </c>
       <c r="C45" t="n">
-        <v>0.243854570213064</v>
+        <v>0.232126120168479</v>
       </c>
       <c r="D45" t="n">
-        <v>0.000000963933405732354</v>
+        <v>0.00000092934547041792</v>
       </c>
       <c r="E45" t="n">
-        <v>0.0000000360665942676465</v>
+        <v>0.0000000706545295820792</v>
       </c>
     </row>
     <row r="46">
@@ -1290,13 +1290,13 @@
         <v>0.23333416</v>
       </c>
       <c r="C46" t="n">
-        <v>0.243084068407775</v>
+        <v>0.230637128485997</v>
       </c>
       <c r="D46" t="n">
-        <v>0.000000964941906763574</v>
+        <v>0.000000931120236484941</v>
       </c>
       <c r="E46" t="n">
-        <v>0.0000000350580932364263</v>
+        <v>0.0000000688797635150591</v>
       </c>
     </row>
     <row r="47">
@@ -1307,13 +1307,13 @@
         <v>0.232445033</v>
       </c>
       <c r="C47" t="n">
-        <v>0.24235499884977</v>
+        <v>0.229219730989055</v>
       </c>
       <c r="D47" t="n">
-        <v>0.000000965896177598544</v>
+        <v>0.000000932809667668907</v>
       </c>
       <c r="E47" t="n">
-        <v>0.0000000341038224014562</v>
+        <v>0.0000000671903323310926</v>
       </c>
     </row>
     <row r="48">
@@ -1324,13 +1324,13 @@
         <v>0.231601522</v>
       </c>
       <c r="C48" t="n">
-        <v>0.241664143712879</v>
+        <v>0.227868980303028</v>
       </c>
       <c r="D48" t="n">
-        <v>0.000000966800430013264</v>
+        <v>0.000000934419660868177</v>
       </c>
       <c r="E48" t="n">
-        <v>0.0000000331995699867362</v>
+        <v>0.0000000655803391318227</v>
       </c>
     </row>
     <row r="49">
@@ -1341,13 +1341,13 @@
         <v>0.230800248</v>
       </c>
       <c r="C49" t="n">
-        <v>0.241008606385855</v>
+        <v>0.226580366047121</v>
       </c>
       <c r="D49" t="n">
-        <v>0.000000967658455349179</v>
+        <v>0.000000935955592117336</v>
       </c>
       <c r="E49" t="n">
-        <v>0.0000000323415446508204</v>
+        <v>0.0000000640444078826638</v>
       </c>
     </row>
     <row r="50">
@@ -1358,13 +1358,13 @@
         <v>0.230038151</v>
       </c>
       <c r="C50" t="n">
-        <v>0.240385772798418</v>
+        <v>0.225349768579521</v>
       </c>
       <c r="D50" t="n">
-        <v>0.000000968473675133087</v>
+        <v>0.000000937422371719501</v>
       </c>
       <c r="E50" t="n">
-        <v>0.000000031526324866913</v>
+        <v>0.000000062577628280499</v>
       </c>
     </row>
     <row r="51">
@@ -1375,13 +1375,13 @@
         <v>0.229312458</v>
       </c>
       <c r="C51" t="n">
-        <v>0.239793278142695</v>
+        <v>0.224173418371351</v>
       </c>
       <c r="D51" t="n">
-        <v>0.000000969249184635061</v>
+        <v>0.000000938824492669507</v>
       </c>
       <c r="E51" t="n">
-        <v>0.0000000307508153649391</v>
+        <v>0.0000000611755073304931</v>
       </c>
     </row>
     <row r="52">
@@ -1392,13 +1392,13 @@
         <v>0.228620648</v>
       </c>
       <c r="C52" t="n">
-        <v>0.239228978141636</v>
+        <v>0.223047860244943</v>
       </c>
       <c r="D52" t="n">
-        <v>0.000000969987790474891</v>
+        <v>0.000000940166073279197</v>
       </c>
       <c r="E52" t="n">
-        <v>0.0000000300122095251094</v>
+        <v>0.0000000598339267208032</v>
       </c>
     </row>
     <row r="53">
@@ -1409,13 +1409,13 @@
         <v>0.227960426</v>
       </c>
       <c r="C53" t="n">
-        <v>0.238690924163362</v>
+        <v>0.221969921825147</v>
       </c>
       <c r="D53" t="n">
-        <v>0.000000970692043194632</v>
+        <v>0.000000941450894781088</v>
       </c>
       <c r="E53" t="n">
-        <v>0.0000000293079568053678</v>
+        <v>0.0000000585491052189118</v>
       </c>
     </row>
     <row r="54">
@@ -1426,13 +1426,13 @@
         <v>0.227329698</v>
       </c>
       <c r="C54" t="n">
-        <v>0.238177341599896</v>
+        <v>0.220936685647698</v>
       </c>
       <c r="D54" t="n">
-        <v>0.000000971364265558444</v>
+        <v>0.000000942682434573102</v>
       </c>
       <c r="E54" t="n">
-        <v>0.0000000286357344415556</v>
+        <v>0.0000000573175654268977</v>
       </c>
     </row>
     <row r="59">
@@ -1457,16 +1457,16 @@
         <v>11</v>
       </c>
       <c r="B60" t="n">
-        <v>24229546.9940493</v>
+        <v>11161490.8152718</v>
       </c>
       <c r="C60" t="n">
         <v>0.000000000000001</v>
       </c>
       <c r="D60" t="n">
-        <v>980306.399515205</v>
+        <v>1011827.570021</v>
       </c>
       <c r="E60" t="n">
-        <v>216299.441230966</v>
+        <v>172848.44474276</v>
       </c>
     </row>
     <row r="61">
@@ -1522,19 +1522,19 @@
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>0.0000431811411794888</v>
+        <v>0.000153293213262929</v>
       </c>
       <c r="B68" t="n">
-        <v>0.00657123589437245</v>
+        <v>0.0123811636473689</v>
       </c>
       <c r="C68" t="n">
-        <v>0.00568664148842454</v>
+        <v>0.00964822691924301</v>
       </c>
       <c r="D68" t="n">
-        <v>0.999271523493237</v>
+        <v>0.992796322462353</v>
       </c>
       <c r="E68" t="n">
-        <v>0.999256656625752</v>
+        <v>0.992649308635055</v>
       </c>
     </row>
     <row r="88">
@@ -1574,7 +1574,7 @@
         <v>40</v>
       </c>
       <c r="E89" t="n">
-        <v>100</v>
+        <v>10000</v>
       </c>
       <c r="F89" t="s">
         <v>26</v>

</xml_diff>